<commit_message>
- Problema do palindromo feito!
</commit_message>
<xml_diff>
--- a/Grafo/doc/casos de teste banco.xlsx
+++ b/Grafo/doc/casos de teste banco.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
   <si>
     <t>CT1</t>
   </si>
@@ -422,12 +422,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FF009900"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -439,19 +439,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -504,25 +491,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -531,18 +516,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF009900"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -851,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AG74"/>
+  <dimension ref="B2:AA74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,10 +860,9 @@
     <col min="20" max="24" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.88671875" customWidth="1"/>
     <col min="27" max="27" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="32" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -926,346 +916,291 @@
       </c>
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
-      <c r="AB2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+    </row>
+    <row r="3" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="J3" s="9" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="J3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="4"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="4"/>
+      <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AA3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-    </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B4" s="8"/>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
       <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="5" t="s">
+      <c r="J4" s="9"/>
+      <c r="K4" s="4" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="1"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="5" t="s">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="T4" s="1"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="5" t="s">
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-    </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B5" s="7"/>
       <c r="C5" s="2">
         <v>3</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="5" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="5" t="s">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="4"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="5" t="s">
+      <c r="X5" s="1"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-    </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B6" s="8"/>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B6" s="7"/>
       <c r="C6" s="2">
         <v>4</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="5" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="4"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="5" t="s">
+      <c r="P6" s="1"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="T6" s="1"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="5" t="s">
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B7" s="7"/>
       <c r="C7" s="2">
         <v>5</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="5" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="5" t="s">
+      <c r="R7" s="11"/>
+      <c r="S7" s="4" t="s">
         <v>33</v>
       </c>
       <c r="T7" s="1"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
       <c r="X7" s="1"/>
-      <c r="Z7" s="12"/>
-      <c r="AA7" s="5" t="s">
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-    </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B8" s="8"/>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
       <c r="C8" s="2">
         <v>6</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="5" t="s">
+      <c r="J8" s="9"/>
+      <c r="K8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="5" t="s">
+      <c r="R8" s="11"/>
+      <c r="S8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="T8" s="1"/>
-      <c r="U8" s="4"/>
+      <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="5" t="s">
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-    </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B9" s="8"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
       <c r="C9" s="2">
         <v>7</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="5" t="s">
+      <c r="J9" s="9"/>
+      <c r="K9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="5" t="s">
+      <c r="R9" s="11"/>
+      <c r="S9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-      <c r="Z9" s="12"/>
-      <c r="AA9" s="5" t="s">
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-    </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
       <c r="C10" s="2">
         <v>8</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="5" t="s">
+      <c r="J10" s="9"/>
+      <c r="K10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="5" t="s">
+      <c r="R10" s="11"/>
+      <c r="S10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="T10" s="1"/>
-      <c r="U10" s="4"/>
+      <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="5" t="s">
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-    </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
       <c r="C11" s="2">
         <v>9</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="7" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="L11" s="1"/>
@@ -1273,8 +1208,8 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="7" t="s">
+      <c r="R11" s="11"/>
+      <c r="S11" s="5" t="s">
         <v>35</v>
       </c>
       <c r="T11" s="1"/>
@@ -1282,113 +1217,98 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="5" t="s">
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-    </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
       <c r="C12" s="2">
         <v>10</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="5" t="s">
+      <c r="J12" s="9"/>
+      <c r="K12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="5" t="s">
+      <c r="R12" s="11"/>
+      <c r="S12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="4"/>
+      <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="5" t="s">
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1"/>
-    </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
       <c r="C13" s="2">
         <v>11</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="5" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="5" t="s">
+      <c r="R13" s="11"/>
+      <c r="S13" s="4" t="s">
         <v>37</v>
       </c>
       <c r="T13" s="1"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="5" t="s">
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
-    </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
       <c r="C14" s="2">
         <v>12</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="5" t="s">
+      <c r="J14" s="9"/>
+      <c r="K14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="4"/>
+      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="7" t="s">
+      <c r="R14" s="11"/>
+      <c r="S14" s="5" t="s">
         <v>38</v>
       </c>
       <c r="T14" s="1"/>
@@ -1396,37 +1316,32 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="5" t="s">
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1"/>
-    </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
       <c r="C15" s="2">
         <v>13</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="5" t="s">
+      <c r="J15" s="9"/>
+      <c r="K15" s="4" t="s">
         <v>27</v>
       </c>
       <c r="L15" s="1"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="7" t="s">
+      <c r="R15" s="11"/>
+      <c r="S15" s="5" t="s">
         <v>39</v>
       </c>
       <c r="T15" s="1"/>
@@ -1434,66 +1349,56 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="5" t="s">
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
-    </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B16" s="7"/>
       <c r="C16" s="2">
         <v>14</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="5" t="s">
+      <c r="J16" s="9"/>
+      <c r="K16" s="4" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="4"/>
+      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="5" t="s">
+      <c r="R16" s="11"/>
+      <c r="S16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="T16" s="1"/>
-      <c r="U16" s="4"/>
+      <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="5" t="s">
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
-    </row>
-    <row r="17" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="J17" s="10"/>
-      <c r="K17" s="5" t="s">
+    </row>
+    <row r="17" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J17" s="9"/>
+      <c r="K17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="4"/>
+      <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="13" t="s">
+      <c r="R17" s="11"/>
+      <c r="S17" s="6" t="s">
         <v>40</v>
       </c>
       <c r="T17" s="1"/>
@@ -1501,760 +1406,469 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="5" t="s">
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="1"/>
-    </row>
-    <row r="18" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="J18" s="10"/>
-      <c r="K18" s="5" t="s">
+    </row>
+    <row r="18" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J18" s="9"/>
+      <c r="K18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="4"/>
+      <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="5" t="s">
+      <c r="R18" s="11"/>
+      <c r="S18" s="4" t="s">
         <v>41</v>
       </c>
       <c r="T18" s="1"/>
-      <c r="U18" s="4"/>
+      <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="5" t="s">
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
-      <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
-    </row>
-    <row r="19" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="J19" s="10"/>
-      <c r="K19" s="5" t="s">
+    </row>
+    <row r="19" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J19" s="9"/>
+      <c r="K19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="4"/>
+      <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="5" t="s">
+      <c r="R19" s="11"/>
+      <c r="S19" s="4" t="s">
         <v>42</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-      <c r="W19" s="4"/>
+      <c r="W19" s="1"/>
       <c r="X19" s="1"/>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="5" t="s">
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="1"/>
-      <c r="AF19" s="1"/>
-    </row>
-    <row r="20" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="J20" s="11"/>
-      <c r="K20" s="5" t="s">
+    </row>
+    <row r="20" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J20" s="10"/>
+      <c r="K20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="R20" s="12"/>
-      <c r="S20" s="5" t="s">
+      <c r="R20" s="11"/>
+      <c r="S20" s="4" t="s">
         <v>43</v>
       </c>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="V20" s="4"/>
+      <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-      <c r="Z20" s="12"/>
-      <c r="AA20" s="5" t="s">
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
-      <c r="AE20" s="1"/>
-      <c r="AF20" s="1"/>
-    </row>
-    <row r="21" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="R21" s="12"/>
-      <c r="S21" s="5" t="s">
+    </row>
+    <row r="21" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="R21" s="11"/>
+      <c r="S21" s="4" t="s">
         <v>44</v>
       </c>
       <c r="T21" s="1"/>
-      <c r="U21" s="4"/>
+      <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="5" t="s">
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-      <c r="AE21" s="1"/>
-      <c r="AF21" s="1"/>
-    </row>
-    <row r="22" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="R22" s="12"/>
-      <c r="S22" s="5" t="s">
+    </row>
+    <row r="22" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="R22" s="11"/>
+      <c r="S22" s="4" t="s">
         <v>45</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
-      <c r="W22" s="4"/>
+      <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="5" t="s">
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
-      <c r="AE22" s="1"/>
-      <c r="AF22" s="1"/>
-    </row>
-    <row r="23" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="R23" s="12"/>
-      <c r="S23" s="5" t="s">
+    </row>
+    <row r="23" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="R23" s="11"/>
+      <c r="S23" s="4" t="s">
         <v>46</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
-      <c r="V23" s="4"/>
+      <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="Z23" s="12"/>
-      <c r="AA23" s="5" t="s">
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
-      <c r="AE23" s="1"/>
-      <c r="AF23" s="1"/>
-    </row>
-    <row r="24" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="R24" s="12"/>
-      <c r="S24" s="5" t="s">
+    </row>
+    <row r="24" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="R24" s="11"/>
+      <c r="S24" s="4" t="s">
         <v>47</v>
       </c>
       <c r="T24" s="1"/>
-      <c r="U24" s="4"/>
+      <c r="U24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-      <c r="Z24" s="12"/>
-      <c r="AA24" s="5" t="s">
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
-      <c r="AE24" s="1"/>
-      <c r="AF24" s="1"/>
-    </row>
-    <row r="25" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="R25" s="12"/>
-      <c r="S25" s="5" t="s">
+    </row>
+    <row r="25" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="R25" s="11"/>
+      <c r="S25" s="4" t="s">
         <v>48</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-      <c r="V25" s="4"/>
+      <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-      <c r="Z25" s="12"/>
-      <c r="AA25" s="5" t="s">
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
-      <c r="AE25" s="1"/>
-      <c r="AF25" s="1"/>
-    </row>
-    <row r="26" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="R26" s="12"/>
-      <c r="S26" s="5" t="s">
+    </row>
+    <row r="26" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="R26" s="11"/>
+      <c r="S26" s="4" t="s">
         <v>49</v>
       </c>
       <c r="T26" s="1"/>
-      <c r="U26" s="4"/>
+      <c r="U26" s="1"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="5" t="s">
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
-      <c r="AE26" s="1"/>
-      <c r="AF26" s="1"/>
-      <c r="AG26" s="1"/>
-    </row>
-    <row r="27" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="R27" s="12"/>
-      <c r="S27" s="5" t="s">
+    </row>
+    <row r="27" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="R27" s="11"/>
+      <c r="S27" s="4" t="s">
         <v>50</v>
       </c>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
       <c r="X27" s="1"/>
-      <c r="Z27" s="12"/>
-      <c r="AA27" s="5" t="s">
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
-      <c r="AF27" s="1"/>
-    </row>
-    <row r="28" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="Z28" s="12"/>
-      <c r="AA28" s="5" t="s">
+    </row>
+    <row r="28" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
-      <c r="AE28" s="1"/>
-      <c r="AF28" s="1"/>
-    </row>
-    <row r="29" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="Z29" s="12"/>
-      <c r="AA29" s="5" t="s">
+    </row>
+    <row r="29" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
-      <c r="AD29" s="1"/>
-      <c r="AE29" s="1"/>
-      <c r="AF29" s="1"/>
-    </row>
-    <row r="30" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="Z30" s="12"/>
-      <c r="AA30" s="5" t="s">
+    </row>
+    <row r="30" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
-      <c r="AE30" s="1"/>
-      <c r="AF30" s="1"/>
-    </row>
-    <row r="31" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="Z31" s="12"/>
-      <c r="AA31" s="5" t="s">
+    </row>
+    <row r="31" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
-      <c r="AE31" s="1"/>
-      <c r="AF31" s="1"/>
-    </row>
-    <row r="32" spans="10:33" x14ac:dyDescent="0.3">
-      <c r="Z32" s="12"/>
-      <c r="AA32" s="5" t="s">
+    </row>
+    <row r="32" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
-      <c r="AE32" s="1"/>
-      <c r="AF32" s="1"/>
-    </row>
-    <row r="33" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z33" s="12"/>
-      <c r="AA33" s="5" t="s">
+    </row>
+    <row r="33" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z33" s="11"/>
+      <c r="AA33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
-      <c r="AE33" s="1"/>
-      <c r="AF33" s="1"/>
-    </row>
-    <row r="34" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z34" s="12"/>
-      <c r="AA34" s="5" t="s">
+    </row>
+    <row r="34" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="1"/>
-      <c r="AE34" s="1"/>
-      <c r="AF34" s="1"/>
-    </row>
-    <row r="35" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z35" s="12"/>
-      <c r="AA35" s="5" t="s">
+    </row>
+    <row r="35" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AB35" s="1"/>
-      <c r="AC35" s="1"/>
-      <c r="AD35" s="1"/>
-      <c r="AE35" s="1"/>
-      <c r="AF35" s="1"/>
-    </row>
-    <row r="36" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z36" s="12"/>
-      <c r="AA36" s="5" t="s">
+    </row>
+    <row r="36" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AB36" s="1"/>
-      <c r="AC36" s="1"/>
-      <c r="AD36" s="1"/>
-      <c r="AE36" s="1"/>
-      <c r="AF36" s="1"/>
-    </row>
-    <row r="37" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z37" s="12"/>
-      <c r="AA37" s="5" t="s">
+    </row>
+    <row r="37" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AB37" s="1"/>
-      <c r="AC37" s="1"/>
-      <c r="AD37" s="1"/>
-      <c r="AE37" s="1"/>
-      <c r="AF37" s="1"/>
-    </row>
-    <row r="38" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z38" s="12"/>
-      <c r="AA38" s="5" t="s">
+    </row>
+    <row r="38" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
-    </row>
-    <row r="39" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z39" s="12"/>
-      <c r="AA39" s="5" t="s">
+    </row>
+    <row r="39" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
-      <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-      <c r="AF39" s="1"/>
-    </row>
-    <row r="40" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z40" s="12"/>
-      <c r="AA40" s="5" t="s">
+    </row>
+    <row r="40" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z40" s="11"/>
+      <c r="AA40" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="AB40" s="1"/>
-      <c r="AC40" s="1"/>
-      <c r="AD40" s="1"/>
-      <c r="AE40" s="1"/>
-      <c r="AF40" s="1"/>
-    </row>
-    <row r="41" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z41" s="12"/>
-      <c r="AA41" s="5" t="s">
+    </row>
+    <row r="41" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z41" s="11"/>
+      <c r="AA41" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="AB41" s="1"/>
-      <c r="AC41" s="1"/>
-      <c r="AD41" s="1"/>
-      <c r="AE41" s="1"/>
-      <c r="AF41" s="1"/>
-    </row>
-    <row r="42" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z42" s="12"/>
-      <c r="AA42" s="5" t="s">
+    </row>
+    <row r="42" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z42" s="11"/>
+      <c r="AA42" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="AB42" s="1"/>
-      <c r="AC42" s="1"/>
-      <c r="AD42" s="1"/>
-      <c r="AE42" s="1"/>
-      <c r="AF42" s="1"/>
-    </row>
-    <row r="43" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z43" s="12"/>
-      <c r="AA43" s="5" t="s">
+    </row>
+    <row r="43" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z43" s="11"/>
+      <c r="AA43" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="1"/>
-      <c r="AD43" s="1"/>
-      <c r="AE43" s="1"/>
-      <c r="AF43" s="1"/>
-    </row>
-    <row r="44" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z44" s="12"/>
-      <c r="AA44" s="5" t="s">
+    </row>
+    <row r="44" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z44" s="11"/>
+      <c r="AA44" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AB44" s="1"/>
-      <c r="AC44" s="1"/>
-      <c r="AD44" s="1"/>
-      <c r="AE44" s="1"/>
-      <c r="AF44" s="1"/>
-    </row>
-    <row r="45" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z45" s="12"/>
-      <c r="AA45" s="5" t="s">
+    </row>
+    <row r="45" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z45" s="11"/>
+      <c r="AA45" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="AB45" s="1"/>
-      <c r="AC45" s="1"/>
-      <c r="AD45" s="1"/>
-      <c r="AE45" s="1"/>
-      <c r="AF45" s="1"/>
-    </row>
-    <row r="46" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z46" s="12"/>
-      <c r="AA46" s="5" t="s">
+    </row>
+    <row r="46" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z46" s="11"/>
+      <c r="AA46" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="AB46" s="1"/>
-      <c r="AC46" s="1"/>
-      <c r="AD46" s="1"/>
-      <c r="AE46" s="1"/>
-      <c r="AF46" s="1"/>
-    </row>
-    <row r="47" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z47" s="12"/>
-      <c r="AA47" s="5" t="s">
+    </row>
+    <row r="47" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z47" s="11"/>
+      <c r="AA47" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AB47" s="1"/>
-      <c r="AC47" s="1"/>
-      <c r="AD47" s="1"/>
-      <c r="AE47" s="1"/>
-      <c r="AF47" s="1"/>
-    </row>
-    <row r="48" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z48" s="12"/>
-      <c r="AA48" s="5" t="s">
+    </row>
+    <row r="48" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z48" s="11"/>
+      <c r="AA48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="AB48" s="1"/>
-      <c r="AC48" s="1"/>
-      <c r="AD48" s="1"/>
-      <c r="AE48" s="1"/>
-      <c r="AF48" s="1"/>
-    </row>
-    <row r="49" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z49" s="12"/>
-      <c r="AA49" s="5" t="s">
+    </row>
+    <row r="49" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z49" s="11"/>
+      <c r="AA49" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
-      <c r="AD49" s="1"/>
-      <c r="AE49" s="1"/>
-      <c r="AF49" s="1"/>
-    </row>
-    <row r="50" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z50" s="12"/>
-      <c r="AA50" s="5" t="s">
+    </row>
+    <row r="50" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z50" s="11"/>
+      <c r="AA50" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
-      <c r="AD50" s="1"/>
-      <c r="AE50" s="1"/>
-      <c r="AF50" s="1"/>
-    </row>
-    <row r="51" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z51" s="12"/>
-      <c r="AA51" s="5" t="s">
+    </row>
+    <row r="51" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z51" s="11"/>
+      <c r="AA51" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AB51" s="1"/>
-      <c r="AC51" s="1"/>
-      <c r="AD51" s="1"/>
-      <c r="AE51" s="1"/>
-      <c r="AF51" s="1"/>
-    </row>
-    <row r="52" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z52" s="12"/>
-      <c r="AA52" s="5" t="s">
+    </row>
+    <row r="52" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z52" s="11"/>
+      <c r="AA52" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="AB52" s="1"/>
-      <c r="AC52" s="1"/>
-      <c r="AD52" s="1"/>
-      <c r="AE52" s="1"/>
-      <c r="AF52" s="1"/>
-    </row>
-    <row r="53" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z53" s="12"/>
-      <c r="AA53" s="5" t="s">
+    </row>
+    <row r="53" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z53" s="11"/>
+      <c r="AA53" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AB53" s="1"/>
-      <c r="AC53" s="1"/>
-      <c r="AD53" s="1"/>
-      <c r="AE53" s="1"/>
-      <c r="AF53" s="1"/>
-    </row>
-    <row r="54" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z54" s="12"/>
-      <c r="AA54" s="5" t="s">
+    </row>
+    <row r="54" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z54" s="11"/>
+      <c r="AA54" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AB54" s="1"/>
-      <c r="AC54" s="1"/>
-      <c r="AD54" s="1"/>
-      <c r="AE54" s="1"/>
-      <c r="AF54" s="1"/>
-    </row>
-    <row r="55" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z55" s="12"/>
-      <c r="AA55" s="5" t="s">
+    </row>
+    <row r="55" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z55" s="11"/>
+      <c r="AA55" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="AB55" s="1"/>
-      <c r="AC55" s="1"/>
-      <c r="AD55" s="1"/>
-      <c r="AE55" s="1"/>
-      <c r="AF55" s="1"/>
-    </row>
-    <row r="56" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z56" s="12"/>
-      <c r="AA56" s="5" t="s">
+    </row>
+    <row r="56" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z56" s="11"/>
+      <c r="AA56" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AB56" s="1"/>
-      <c r="AC56" s="1"/>
-      <c r="AD56" s="1"/>
-      <c r="AE56" s="1"/>
-      <c r="AF56" s="1"/>
-    </row>
-    <row r="57" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z57" s="12"/>
-      <c r="AA57" s="5" t="s">
+    </row>
+    <row r="57" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z57" s="11"/>
+      <c r="AA57" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AB57" s="1"/>
-      <c r="AC57" s="1"/>
-      <c r="AD57" s="1"/>
-      <c r="AE57" s="1"/>
-      <c r="AF57" s="1"/>
-    </row>
-    <row r="58" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z58" s="12"/>
-      <c r="AA58" s="5" t="s">
+    </row>
+    <row r="58" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z58" s="11"/>
+      <c r="AA58" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AB58" s="1"/>
-      <c r="AC58" s="1"/>
-      <c r="AD58" s="1"/>
-      <c r="AE58" s="1"/>
-      <c r="AF58" s="1"/>
-    </row>
-    <row r="59" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z59" s="12"/>
-      <c r="AA59" s="5" t="s">
+    </row>
+    <row r="59" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z59" s="11"/>
+      <c r="AA59" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AB59" s="1"/>
-      <c r="AC59" s="1"/>
-      <c r="AD59" s="1"/>
-      <c r="AE59" s="1"/>
-      <c r="AF59" s="1"/>
-    </row>
-    <row r="60" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z60" s="12"/>
-      <c r="AA60" s="5" t="s">
+    </row>
+    <row r="60" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z60" s="11"/>
+      <c r="AA60" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AB60" s="1"/>
-      <c r="AC60" s="1"/>
-      <c r="AD60" s="1"/>
-      <c r="AE60" s="1"/>
-      <c r="AF60" s="1"/>
-    </row>
-    <row r="61" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z61" s="12"/>
-      <c r="AA61" s="5" t="s">
+    </row>
+    <row r="61" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z61" s="11"/>
+      <c r="AA61" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AB61" s="1"/>
-      <c r="AC61" s="1"/>
-      <c r="AD61" s="1"/>
-      <c r="AE61" s="1"/>
-      <c r="AF61" s="1"/>
-    </row>
-    <row r="62" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z62" s="12"/>
-      <c r="AA62" s="5" t="s">
+    </row>
+    <row r="62" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z62" s="11"/>
+      <c r="AA62" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AB62" s="1"/>
-      <c r="AC62" s="1"/>
-      <c r="AD62" s="1"/>
-      <c r="AE62" s="1"/>
-      <c r="AF62" s="1"/>
-    </row>
-    <row r="63" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z63" s="12"/>
-      <c r="AA63" s="5" t="s">
+    </row>
+    <row r="63" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z63" s="11"/>
+      <c r="AA63" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AB63" s="1"/>
-      <c r="AC63" s="1"/>
-      <c r="AD63" s="1"/>
-      <c r="AE63" s="1"/>
-      <c r="AF63" s="1"/>
-    </row>
-    <row r="64" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z64" s="12"/>
-      <c r="AA64" s="5" t="s">
+    </row>
+    <row r="64" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z64" s="11"/>
+      <c r="AA64" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AB64" s="1"/>
-      <c r="AC64" s="1"/>
-      <c r="AD64" s="1"/>
-      <c r="AE64" s="1"/>
-      <c r="AF64" s="1"/>
-    </row>
-    <row r="65" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z65" s="12"/>
-      <c r="AA65" s="5" t="s">
+    </row>
+    <row r="65" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z65" s="11"/>
+      <c r="AA65" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AB65" s="1"/>
-      <c r="AC65" s="1"/>
-      <c r="AD65" s="1"/>
-      <c r="AE65" s="1"/>
-      <c r="AF65" s="1"/>
-    </row>
-    <row r="66" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z66" s="12"/>
-      <c r="AA66" s="5" t="s">
+    </row>
+    <row r="66" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z66" s="11"/>
+      <c r="AA66" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AB66" s="1"/>
-      <c r="AC66" s="1"/>
-      <c r="AD66" s="1"/>
-      <c r="AE66" s="1"/>
-      <c r="AF66" s="1"/>
-    </row>
-    <row r="67" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z67" s="12"/>
-      <c r="AA67" s="5" t="s">
+    </row>
+    <row r="67" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z67" s="11"/>
+      <c r="AA67" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="1"/>
-      <c r="AD67" s="1"/>
-      <c r="AE67" s="1"/>
-      <c r="AF67" s="1"/>
-    </row>
-    <row r="68" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z68" s="12"/>
-      <c r="AA68" s="5" t="s">
+    </row>
+    <row r="68" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z68" s="11"/>
+      <c r="AA68" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AB68" s="1"/>
-      <c r="AC68" s="1"/>
-      <c r="AD68" s="1"/>
-      <c r="AE68" s="1"/>
-      <c r="AF68" s="1"/>
-    </row>
-    <row r="69" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z69" s="12"/>
-      <c r="AA69" s="5" t="s">
+    </row>
+    <row r="69" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z69" s="11"/>
+      <c r="AA69" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="AB69" s="1"/>
-      <c r="AC69" s="1"/>
-      <c r="AD69" s="1"/>
-      <c r="AE69" s="1"/>
-      <c r="AF69" s="1"/>
-    </row>
-    <row r="70" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z70" s="12"/>
-      <c r="AA70" s="5" t="s">
+    </row>
+    <row r="70" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z70" s="11"/>
+      <c r="AA70" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="AB70" s="1"/>
-      <c r="AC70" s="1"/>
-      <c r="AD70" s="1"/>
-      <c r="AE70" s="1"/>
-      <c r="AF70" s="1"/>
-    </row>
-    <row r="71" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z71" s="12"/>
-      <c r="AA71" s="5" t="s">
+    </row>
+    <row r="71" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z71" s="11"/>
+      <c r="AA71" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="AB71" s="1"/>
-      <c r="AC71" s="1"/>
-      <c r="AD71" s="1"/>
-      <c r="AE71" s="1"/>
-      <c r="AF71" s="1"/>
-    </row>
-    <row r="72" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z72" s="12"/>
-      <c r="AA72" s="5" t="s">
+    </row>
+    <row r="72" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z72" s="11"/>
+      <c r="AA72" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="AB72" s="1"/>
-      <c r="AC72" s="1"/>
-      <c r="AD72" s="1"/>
-      <c r="AE72" s="1"/>
-      <c r="AF72" s="1"/>
-    </row>
-    <row r="73" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z73" s="12"/>
-      <c r="AA73" s="5" t="s">
+    </row>
+    <row r="73" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z73" s="11"/>
+      <c r="AA73" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="AB73" s="1"/>
-      <c r="AC73" s="1"/>
-      <c r="AD73" s="1"/>
-      <c r="AE73" s="1"/>
-      <c r="AF73" s="1"/>
-    </row>
-    <row r="74" spans="26:32" x14ac:dyDescent="0.3">
-      <c r="Z74" s="12"/>
-      <c r="AA74" s="5" t="s">
+    </row>
+    <row r="74" spans="26:27" x14ac:dyDescent="0.3">
+      <c r="Z74" s="11"/>
+      <c r="AA74" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AB74" s="1"/>
-      <c r="AC74" s="1"/>
-      <c r="AD74" s="1"/>
-      <c r="AE74" s="1"/>
-      <c r="AF74" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>